<commit_message>
Revert "Removed extra columns"
This reverts commit 8ca90dbb627db303d3e625d0aeb620e796b7c5dd.
</commit_message>
<xml_diff>
--- a/Data/ResponseVariables.xlsx
+++ b/Data/ResponseVariables.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\NC_DMS2\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WorkSpace\EEP_Tool\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="206">
   <si>
     <t>variable</t>
   </si>
@@ -1303,7 +1303,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1313,6 +1312,7 @@
     <xf numFmtId="0" fontId="16" fillId="36" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1643,7 +1643,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1666,11 +1666,11 @@
       <c r="C1" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="22" t="s">
         <v>177</v>
       </c>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -1735,7 +1735,7 @@
       <c r="B5" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="20" t="s">
         <v>191</v>
       </c>
       <c r="E5" s="8" t="s">
@@ -1756,7 +1756,7 @@
       <c r="B6" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="C6" s="22"/>
+      <c r="C6" s="21"/>
       <c r="E6" s="8" t="s">
         <v>195</v>
       </c>
@@ -1775,7 +1775,7 @@
       <c r="B7" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="C7" s="22"/>
+      <c r="C7" s="21"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
@@ -1784,7 +1784,7 @@
       <c r="B8" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="C8" s="22"/>
+      <c r="C8" s="21"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
@@ -1793,7 +1793,7 @@
       <c r="B9" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="C9" s="22"/>
+      <c r="C9" s="21"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
@@ -1802,7 +1802,7 @@
       <c r="B10" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="C10" s="22"/>
+      <c r="C10" s="21"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
@@ -1811,7 +1811,7 @@
       <c r="B11" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="C11" s="22"/>
+      <c r="C11" s="21"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
@@ -1820,7 +1820,7 @@
       <c r="B12" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="C12" s="22"/>
+      <c r="C12" s="21"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
@@ -1834,18 +1834,18 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="23" t="s">
         <v>197</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="23" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="23" t="s">
         <v>203</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="23" t="s">
         <v>205</v>
       </c>
     </row>
@@ -1867,10 +1867,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M80"/>
+  <dimension ref="A1:N80"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:N1048576"/>
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1879,9 +1879,10 @@
     <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="92.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="12" width="9.140625" style="2"/>
+    <col min="14" max="14" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>192</v>
       </c>
@@ -1921,8 +1922,11 @@
       <c r="M1" s="15" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N1" s="15" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1946,8 +1950,12 @@
       <c r="M2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N2">
+        <f>M2*10+L2</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1971,8 +1979,12 @@
       <c r="M3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N3">
+        <f t="shared" ref="N3:N66" si="0">M3*10+L3</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1996,8 +2008,12 @@
       <c r="M4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N4">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2021,8 +2037,12 @@
       <c r="M5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N5">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -2046,8 +2066,12 @@
       <c r="M6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -2071,8 +2095,12 @@
       <c r="M7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -2096,8 +2124,12 @@
       <c r="M8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N8">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -2121,8 +2153,12 @@
       <c r="M9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N9">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -2141,8 +2177,12 @@
       <c r="M10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N10">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -2161,8 +2201,12 @@
       <c r="M11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N11">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -2181,8 +2225,12 @@
       <c r="M12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N12">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -2201,8 +2249,12 @@
       <c r="M13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="N13">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -2226,8 +2278,12 @@
       <c r="M14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="N14">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="16">
         <v>14</v>
       </c>
@@ -2251,8 +2307,12 @@
       <c r="M15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="N15">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="16">
         <v>15</v>
       </c>
@@ -2276,8 +2336,12 @@
       <c r="M16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N16">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -2296,8 +2360,12 @@
       <c r="M17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N17">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -2316,8 +2384,12 @@
       <c r="M18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N18">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -2336,8 +2408,12 @@
       <c r="M19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N19">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -2356,8 +2432,12 @@
       <c r="M20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N20">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -2376,8 +2456,12 @@
       <c r="M21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N21">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -2396,8 +2480,12 @@
       <c r="M22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="N22">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -2421,8 +2509,12 @@
       <c r="M23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="N23">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -2446,8 +2538,12 @@
       <c r="M24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="N24">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -2471,8 +2567,12 @@
       <c r="M25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="N25">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -2496,8 +2596,12 @@
       <c r="M26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N26">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -2513,8 +2617,12 @@
       <c r="M27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N27">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -2530,8 +2638,12 @@
       <c r="M28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N28">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -2547,8 +2659,12 @@
       <c r="M29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N29">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -2564,8 +2680,12 @@
       <c r="M30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N30">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -2587,8 +2707,12 @@
       <c r="M31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N31">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -2610,8 +2734,12 @@
       <c r="M32">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N32">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -2633,8 +2761,12 @@
       <c r="M33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N33">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -2656,8 +2788,12 @@
       <c r="M34">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N34">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -2679,8 +2815,12 @@
       <c r="M35">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N35">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -2702,8 +2842,12 @@
       <c r="M36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N36">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -2725,8 +2869,12 @@
       <c r="M37">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N37">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -2742,8 +2890,12 @@
       <c r="M38">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N38">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -2765,8 +2917,12 @@
       <c r="M39">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N39">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -2788,8 +2944,12 @@
       <c r="M40">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N40">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -2811,8 +2971,12 @@
       <c r="M41">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N41">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -2834,8 +2998,12 @@
       <c r="M42">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N42">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -2857,8 +3025,12 @@
       <c r="M43">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N43">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -2880,8 +3052,12 @@
       <c r="M44">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N44">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -2903,8 +3079,12 @@
       <c r="M45">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N45">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -2920,8 +3100,12 @@
       <c r="M46">
         <v>2</v>
       </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N46">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -2943,8 +3127,12 @@
       <c r="M47">
         <v>2</v>
       </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N47">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -2969,8 +3157,12 @@
       <c r="M48">
         <v>2</v>
       </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N48">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -2995,8 +3187,12 @@
       <c r="M49">
         <v>2</v>
       </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N49">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -3021,8 +3217,12 @@
       <c r="M50">
         <v>2</v>
       </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N50">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -3047,8 +3247,12 @@
       <c r="M51">
         <v>2</v>
       </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N51">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -3073,8 +3277,12 @@
       <c r="M52">
         <v>2</v>
       </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N52">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -3096,8 +3304,12 @@
       <c r="M53">
         <v>2</v>
       </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N53">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -3113,8 +3325,12 @@
       <c r="M54">
         <v>2</v>
       </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N54">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -3133,8 +3349,12 @@
       <c r="M55">
         <v>2</v>
       </c>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N55">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -3157,8 +3377,12 @@
       <c r="M56">
         <v>2</v>
       </c>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N56">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -3181,8 +3405,12 @@
       <c r="M57">
         <v>2</v>
       </c>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N57">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -3205,8 +3433,12 @@
       <c r="M58">
         <v>2</v>
       </c>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N58">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -3229,8 +3461,12 @@
       <c r="M59">
         <v>2</v>
       </c>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N59">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>59</v>
       </c>
@@ -3253,8 +3489,12 @@
       <c r="M60">
         <v>2</v>
       </c>
-    </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N60">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>60</v>
       </c>
@@ -3277,8 +3517,12 @@
       <c r="M61">
         <v>2</v>
       </c>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N61">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>61</v>
       </c>
@@ -3295,8 +3539,12 @@
       <c r="M62">
         <v>2</v>
       </c>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N62">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>62</v>
       </c>
@@ -3316,8 +3564,12 @@
       <c r="M63">
         <v>2</v>
       </c>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N63">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>63</v>
       </c>
@@ -3340,8 +3592,12 @@
       <c r="M64">
         <v>2</v>
       </c>
-    </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N64">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>64</v>
       </c>
@@ -3364,8 +3620,12 @@
       <c r="M65">
         <v>2</v>
       </c>
-    </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N65">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>65</v>
       </c>
@@ -3388,8 +3648,12 @@
       <c r="M66">
         <v>2</v>
       </c>
-    </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N66">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>66</v>
       </c>
@@ -3412,8 +3676,12 @@
       <c r="M67">
         <v>2</v>
       </c>
-    </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N67">
+        <f t="shared" ref="N67:N80" si="1">M67*10+L67</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>67</v>
       </c>
@@ -3436,8 +3704,12 @@
       <c r="M68">
         <v>2</v>
       </c>
-    </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N68">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>68</v>
       </c>
@@ -3460,8 +3732,12 @@
       <c r="M69">
         <v>2</v>
       </c>
-    </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N69">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>69</v>
       </c>
@@ -3480,8 +3756,12 @@
       <c r="M70">
         <v>2</v>
       </c>
-    </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N70">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>70</v>
       </c>
@@ -3500,8 +3780,12 @@
       <c r="M71">
         <v>2</v>
       </c>
-    </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N71">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>71</v>
       </c>
@@ -3520,8 +3804,12 @@
       <c r="M72">
         <v>1</v>
       </c>
-    </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N72">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>72</v>
       </c>
@@ -3540,8 +3828,12 @@
       <c r="M73">
         <v>1</v>
       </c>
-    </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N73">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>73</v>
       </c>
@@ -3560,8 +3852,12 @@
       <c r="M74">
         <v>1</v>
       </c>
-    </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N74">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>74</v>
       </c>
@@ -3577,8 +3873,12 @@
       <c r="M75">
         <v>1</v>
       </c>
-    </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N75">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>75</v>
       </c>
@@ -3594,8 +3894,12 @@
       <c r="M76">
         <v>1</v>
       </c>
-    </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N76">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>76</v>
       </c>
@@ -3614,8 +3918,12 @@
       <c r="M77">
         <v>2</v>
       </c>
-    </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N77">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>77</v>
       </c>
@@ -3634,8 +3942,12 @@
       <c r="M78">
         <v>2</v>
       </c>
-    </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N78">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>78</v>
       </c>
@@ -3654,8 +3966,12 @@
       <c r="M79">
         <v>2</v>
       </c>
-    </row>
-    <row r="80" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N79">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>79</v>
       </c>
@@ -3673,6 +3989,10 @@
       </c>
       <c r="M80">
         <v>2</v>
+      </c>
+      <c r="N80">
+        <f t="shared" si="1"/>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>